<commit_message>
add some more files
</commit_message>
<xml_diff>
--- a/nj property tax over time.xlsx
+++ b/nj property tax over time.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Year 1</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>7 Robinwood</t>
   </si>
 </sst>
 </file>
@@ -389,20 +392,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -412,14 +414,20 @@
       <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H1" t="s">
         <v>13</v>
       </c>
       <c r="I1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -432,14 +440,20 @@
       <c r="D2">
         <v>15000</v>
       </c>
+      <c r="G2">
+        <v>13058</v>
+      </c>
       <c r="H2">
         <v>14611</v>
       </c>
       <c r="I2">
         <v>14880</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>15850</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -452,14 +466,20 @@
       <c r="D3">
         <v>15300</v>
       </c>
+      <c r="G3">
+        <v>13358</v>
+      </c>
       <c r="H3">
         <v>14911</v>
       </c>
       <c r="I3">
         <v>15180</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>16150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -472,14 +492,20 @@
       <c r="D4">
         <v>15600</v>
       </c>
+      <c r="G4">
+        <v>13658</v>
+      </c>
       <c r="H4">
         <v>15211</v>
       </c>
       <c r="I4">
         <v>15480</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>16450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -492,14 +518,20 @@
       <c r="D5">
         <v>15900</v>
       </c>
+      <c r="G5">
+        <v>13958</v>
+      </c>
       <c r="H5">
         <v>15511</v>
       </c>
       <c r="I5">
         <v>15780</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>16750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -512,14 +544,20 @@
       <c r="D6">
         <v>16200</v>
       </c>
+      <c r="G6">
+        <v>14258</v>
+      </c>
       <c r="H6">
         <v>15811</v>
       </c>
       <c r="I6">
         <v>16080</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>17050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -532,14 +570,20 @@
       <c r="D7">
         <v>16500</v>
       </c>
+      <c r="G7">
+        <v>14558</v>
+      </c>
       <c r="H7">
         <v>16111</v>
       </c>
       <c r="I7">
         <v>16380</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>17350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -552,14 +596,20 @@
       <c r="D8">
         <v>16800</v>
       </c>
+      <c r="G8">
+        <v>14858</v>
+      </c>
       <c r="H8">
         <v>16411</v>
       </c>
       <c r="I8">
         <v>16680</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>17650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -572,14 +622,20 @@
       <c r="D9">
         <v>17100</v>
       </c>
+      <c r="G9">
+        <v>15158</v>
+      </c>
       <c r="H9">
         <v>16711</v>
       </c>
       <c r="I9">
         <v>16980</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>17950</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -592,14 +648,20 @@
       <c r="D10">
         <v>17400</v>
       </c>
+      <c r="G10">
+        <v>15458</v>
+      </c>
       <c r="H10">
         <v>17011</v>
       </c>
       <c r="I10">
         <v>17280</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>18250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -612,14 +674,20 @@
       <c r="D11">
         <v>17700</v>
       </c>
+      <c r="G11">
+        <v>15758</v>
+      </c>
       <c r="H11">
         <v>17311</v>
       </c>
       <c r="I11">
         <v>17580</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>18550</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -635,6 +703,10 @@
         <f>AVERAGE(D2:D12)</f>
         <v>16350</v>
       </c>
+      <c r="G13">
+        <f>AVERAGE(G2:G12)</f>
+        <v>14408</v>
+      </c>
       <c r="H13">
         <f>AVERAGE(H2:H12)</f>
         <v>15961</v>
@@ -642,6 +714,10 @@
       <c r="I13">
         <f>AVERAGE(I2:I12)</f>
         <v>16230</v>
+      </c>
+      <c r="J13">
+        <f>AVERAGE(J2:J12)</f>
+        <v>17200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>